<commit_message>
fix sales prices & deleted traffic dataset
</commit_message>
<xml_diff>
--- a/sales_prices.xlsx
+++ b/sales_prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samav\Documents\fanniemae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97E6225-BDE0-4EAF-8D07-49E7EDFF8F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70225A5-DF80-4AFB-ABAE-4E044D97D175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9EEF5B4F-0E4F-41D9-A974-8F46C70F992C}"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="7810" xr2:uid="{9EEF5B4F-0E4F-41D9-A974-8F46C70F992C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Prices" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -652,6 +652,13 @@
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -974,13 +981,13 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" style="19" customWidth="1"/>
     <col min="3" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="19" width="12.1796875" bestFit="1" customWidth="1"/>
@@ -1026,7 +1033,7 @@
       <c r="A1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>142</v>
       </c>
       <c r="C1" s="4"/>
@@ -1153,7 +1160,7 @@
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="18">
         <f>AVERAGE(CT2:DA2)</f>
         <v>281093.75</v>
       </c>
@@ -1265,7 +1272,7 @@
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="18">
         <f t="shared" ref="B3:B66" si="0">AVERAGE(CT3:DA3)</f>
         <v>532032.25</v>
       </c>
@@ -1377,7 +1384,7 @@
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="18">
         <f t="shared" si="0"/>
         <v>687406.125</v>
       </c>
@@ -1489,7 +1496,7 @@
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="18">
         <f t="shared" si="0"/>
         <v>146800</v>
       </c>
@@ -1601,7 +1608,7 @@
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="18">
         <f t="shared" si="0"/>
         <v>320800</v>
       </c>
@@ -1713,7 +1720,7 @@
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="18">
         <f t="shared" si="0"/>
         <v>262843.75</v>
       </c>
@@ -1825,7 +1832,7 @@
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="18">
         <f t="shared" si="0"/>
         <v>285262.5</v>
       </c>
@@ -1937,7 +1944,7 @@
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="18">
         <f t="shared" si="0"/>
         <v>723656.25</v>
       </c>
@@ -2049,7 +2056,7 @@
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="18">
         <f t="shared" si="0"/>
         <v>335393.75</v>
       </c>
@@ -2161,7 +2168,7 @@
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="18">
         <f t="shared" si="0"/>
         <v>301187.5</v>
       </c>
@@ -2273,7 +2280,7 @@
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="18">
         <f t="shared" si="0"/>
         <v>373815.625</v>
       </c>
@@ -2386,7 +2393,7 @@
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>171456.25</v>
       </c>
@@ -2498,7 +2505,7 @@
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>352440.625</v>
       </c>
@@ -2610,7 +2617,7 @@
       <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>188081.25</v>
       </c>
@@ -2722,7 +2729,7 @@
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>191586.875</v>
       </c>
@@ -2834,7 +2841,7 @@
       <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="18">
         <f t="shared" si="0"/>
         <v>105359.375</v>
       </c>
@@ -2946,7 +2953,7 @@
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="18">
         <f t="shared" si="0"/>
         <v>256750</v>
       </c>
@@ -3058,7 +3065,7 @@
       <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="18">
         <f t="shared" si="0"/>
         <v>196400</v>
       </c>
@@ -3170,7 +3177,7 @@
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="18">
         <f t="shared" si="0"/>
         <v>280893.75</v>
       </c>
@@ -3282,7 +3289,7 @@
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="18">
         <f t="shared" si="0"/>
         <v>360106.25</v>
       </c>
@@ -3394,7 +3401,7 @@
       <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="18">
         <f t="shared" si="0"/>
         <v>208334.375</v>
       </c>
@@ -3506,7 +3513,7 @@
       <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="18">
         <f t="shared" si="0"/>
         <v>295000</v>
       </c>
@@ -3618,7 +3625,7 @@
       <c r="A24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="18">
         <f t="shared" si="0"/>
         <v>200462.5</v>
       </c>
@@ -3730,7 +3737,7 @@
       <c r="A25" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="18">
         <f t="shared" si="0"/>
         <v>519781.25</v>
       </c>
@@ -3842,7 +3849,7 @@
       <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="18">
         <f t="shared" si="0"/>
         <v>383993.75</v>
       </c>
@@ -3954,7 +3961,7 @@
       <c r="A27" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="18">
         <f t="shared" si="0"/>
         <v>413434.375</v>
       </c>
@@ -4066,7 +4073,7 @@
       <c r="A28" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="18">
         <f t="shared" si="0"/>
         <v>512556.25</v>
       </c>
@@ -4178,7 +4185,7 @@
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="18">
         <f t="shared" si="0"/>
         <v>272233.375</v>
       </c>
@@ -4290,7 +4297,7 @@
       <c r="A30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="18">
         <f t="shared" si="0"/>
         <v>146306.25</v>
       </c>
@@ -4402,7 +4409,7 @@
       <c r="A31" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="18">
         <f t="shared" si="0"/>
         <v>312534.375</v>
       </c>
@@ -4514,7 +4521,7 @@
       <c r="A32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="18">
         <f t="shared" si="0"/>
         <v>480381.875</v>
       </c>
@@ -4626,7 +4633,7 @@
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="18">
         <f t="shared" si="0"/>
         <v>289106.25</v>
       </c>
@@ -4738,7 +4745,7 @@
       <c r="A34" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="18">
         <f t="shared" si="0"/>
         <v>150518.75</v>
       </c>
@@ -4850,7 +4857,7 @@
       <c r="A35" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="18">
         <f t="shared" si="0"/>
         <v>135464.28571428571</v>
       </c>
@@ -4962,7 +4969,7 @@
       <c r="A36" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="18">
         <f t="shared" si="0"/>
         <v>289062.5</v>
       </c>
@@ -5074,7 +5081,7 @@
       <c r="A37" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="18">
         <f t="shared" si="0"/>
         <v>170833.33333333334</v>
       </c>
@@ -5186,7 +5193,7 @@
       <c r="A38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="18">
         <f t="shared" si="0"/>
         <v>327743.875</v>
       </c>
@@ -5298,7 +5305,7 @@
       <c r="A39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="18">
         <f t="shared" si="0"/>
         <v>747031.25</v>
       </c>
@@ -5410,7 +5417,7 @@
       <c r="A40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="18">
         <f t="shared" si="0"/>
         <v>731956.25</v>
       </c>
@@ -5522,7 +5529,7 @@
       <c r="A41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="18">
         <f>AVERAGE(CT41:DA41)</f>
         <v>1043750</v>
       </c>
@@ -5634,7 +5641,7 @@
       <c r="A42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="18">
         <f t="shared" si="0"/>
         <v>589531.25</v>
       </c>
@@ -5746,7 +5753,7 @@
       <c r="A43" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="18">
         <f t="shared" si="0"/>
         <v>268762.5</v>
       </c>
@@ -5858,7 +5865,7 @@
       <c r="A44" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="18">
         <f t="shared" si="0"/>
         <v>347996.375</v>
       </c>
@@ -5970,7 +5977,7 @@
       <c r="A45" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="18">
         <f t="shared" si="0"/>
         <v>285514.375</v>
       </c>
@@ -6082,7 +6089,7 @@
       <c r="A46" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="18">
         <f t="shared" si="0"/>
         <v>369356.375</v>
       </c>
@@ -6194,7 +6201,7 @@
       <c r="A47" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="18">
         <f t="shared" si="0"/>
         <v>423336.25</v>
       </c>
@@ -6306,7 +6313,7 @@
       <c r="A48" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="18">
         <f t="shared" si="0"/>
         <v>450987.5</v>
       </c>
@@ -6418,7 +6425,7 @@
       <c r="A49" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="18">
         <f t="shared" si="0"/>
         <v>165028.125</v>
       </c>
@@ -6530,7 +6537,7 @@
       <c r="A50" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" s="18">
         <f t="shared" si="0"/>
         <v>192042.25</v>
       </c>
@@ -6642,7 +6649,7 @@
       <c r="A51" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="18">
         <f t="shared" si="0"/>
         <v>348598.5</v>
       </c>
@@ -6754,7 +6761,7 @@
       <c r="A52" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="18">
         <f t="shared" si="0"/>
         <v>632318.375</v>
       </c>
@@ -6866,7 +6873,7 @@
       <c r="A53" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="18">
         <f t="shared" si="0"/>
         <v>192718.75</v>
       </c>
@@ -6978,7 +6985,7 @@
       <c r="A54" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="18">
         <f t="shared" si="0"/>
         <v>398769.375</v>
       </c>
@@ -7090,7 +7097,7 @@
       <c r="A55" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="18">
         <f t="shared" si="0"/>
         <v>166500</v>
       </c>
@@ -7202,7 +7209,7 @@
       <c r="A56" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56" s="18">
         <f t="shared" si="0"/>
         <v>178687.5</v>
       </c>
@@ -7314,7 +7321,7 @@
       <c r="A57" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57" s="18">
         <f t="shared" si="0"/>
         <v>274407.875</v>
       </c>
@@ -7426,7 +7433,7 @@
       <c r="A58" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58" s="18">
         <f t="shared" si="0"/>
         <v>472275</v>
       </c>
@@ -7538,7 +7545,7 @@
       <c r="A59" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="18">
         <f t="shared" si="0"/>
         <v>285354.5</v>
       </c>
@@ -7650,7 +7657,7 @@
       <c r="A60" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="18">
         <f t="shared" si="0"/>
         <v>392421.25</v>
       </c>
@@ -7762,7 +7769,7 @@
       <c r="A61" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61" s="18">
         <f t="shared" si="0"/>
         <v>167375</v>
       </c>
@@ -7874,7 +7881,7 @@
       <c r="A62" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="18">
         <f t="shared" si="0"/>
         <v>414168.75</v>
       </c>
@@ -7986,7 +7993,7 @@
       <c r="A63" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B63" s="18">
         <f t="shared" si="0"/>
         <v>231109.375</v>
       </c>
@@ -8098,7 +8105,7 @@
       <c r="A64" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64" s="18">
         <f t="shared" si="0"/>
         <v>389039.125</v>
       </c>
@@ -8210,7 +8217,7 @@
       <c r="A65" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="18">
         <f t="shared" si="0"/>
         <v>450875</v>
       </c>
@@ -8322,7 +8329,7 @@
       <c r="A66" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="18">
         <f t="shared" si="0"/>
         <v>287981.25</v>
       </c>
@@ -8434,7 +8441,7 @@
       <c r="A67" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B67" s="18">
         <f t="shared" ref="B67:B130" si="1">AVERAGE(CT67:DA67)</f>
         <v>471018.625</v>
       </c>
@@ -8546,7 +8553,7 @@
       <c r="A68" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B68" s="18">
         <f t="shared" si="1"/>
         <v>350324</v>
       </c>
@@ -8658,7 +8665,7 @@
       <c r="A69" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="18">
         <f t="shared" si="1"/>
         <v>409155.375</v>
       </c>
@@ -8770,7 +8777,7 @@
       <c r="A70" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B70" s="18">
         <f t="shared" si="1"/>
         <v>148406.25</v>
       </c>
@@ -8882,7 +8889,7 @@
       <c r="A71" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B71" s="8">
+      <c r="B71" s="18">
         <f t="shared" si="1"/>
         <v>448312.5</v>
       </c>
@@ -8994,7 +9001,7 @@
       <c r="A72" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="8">
+      <c r="B72" s="18">
         <f t="shared" si="1"/>
         <v>734564.125</v>
       </c>
@@ -9106,7 +9113,7 @@
       <c r="A73" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B73" s="18">
         <f t="shared" si="1"/>
         <v>392934.5</v>
       </c>
@@ -9218,7 +9225,7 @@
       <c r="A74" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B74" s="8">
+      <c r="B74" s="18">
         <f t="shared" si="1"/>
         <v>202512.5</v>
       </c>
@@ -9330,7 +9337,7 @@
       <c r="A75" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B75" s="18">
         <f t="shared" si="1"/>
         <v>272562.5</v>
       </c>
@@ -9442,7 +9449,7 @@
       <c r="A76" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B76" s="8">
+      <c r="B76" s="18">
         <f t="shared" si="1"/>
         <v>418613.25</v>
       </c>
@@ -9554,7 +9561,7 @@
       <c r="A77" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="18">
         <f t="shared" si="1"/>
         <v>448972.125</v>
       </c>
@@ -9666,7 +9673,7 @@
       <c r="A78" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B78" s="18">
         <f t="shared" si="1"/>
         <v>450943.75</v>
       </c>
@@ -9778,7 +9785,7 @@
       <c r="A79" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="18">
         <f t="shared" si="1"/>
         <v>142515.625</v>
       </c>
@@ -9890,7 +9897,7 @@
       <c r="A80" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="8">
+      <c r="B80" s="18">
         <f t="shared" si="1"/>
         <v>373656.25</v>
       </c>
@@ -10002,7 +10009,7 @@
       <c r="A81" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="8">
+      <c r="B81" s="18">
         <f t="shared" si="1"/>
         <v>294106.25</v>
       </c>
@@ -10114,7 +10121,7 @@
       <c r="A82" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B82" s="8">
+      <c r="B82" s="18">
         <f t="shared" si="1"/>
         <v>365175</v>
       </c>
@@ -10226,7 +10233,7 @@
       <c r="A83" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B83" s="18">
         <f t="shared" si="1"/>
         <v>342113</v>
       </c>
@@ -10338,7 +10345,7 @@
       <c r="A84" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B84" s="8">
+      <c r="B84" s="18">
         <f t="shared" si="1"/>
         <v>402309.375</v>
       </c>
@@ -10450,7 +10457,7 @@
       <c r="A85" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B85" s="18">
         <f t="shared" si="1"/>
         <v>442422.25</v>
       </c>
@@ -10562,7 +10569,7 @@
       <c r="A86" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="18">
         <f t="shared" si="1"/>
         <v>287137.5</v>
       </c>
@@ -10674,7 +10681,7 @@
       <c r="A87" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="8">
+      <c r="B87" s="18">
         <f t="shared" si="1"/>
         <v>306593.75</v>
       </c>
@@ -10786,7 +10793,7 @@
       <c r="A88" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B88" s="8">
+      <c r="B88" s="18">
         <f t="shared" si="1"/>
         <v>445903.125</v>
       </c>
@@ -10898,7 +10905,7 @@
       <c r="A89" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B89" s="8">
+      <c r="B89" s="18">
         <f t="shared" si="1"/>
         <v>431559.375</v>
       </c>
@@ -11010,7 +11017,7 @@
       <c r="A90" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B90" s="8">
+      <c r="B90" s="18">
         <f t="shared" si="1"/>
         <v>133719.5</v>
       </c>
@@ -11122,7 +11129,7 @@
       <c r="A91" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B91" s="8">
+      <c r="B91" s="18">
         <f t="shared" si="1"/>
         <v>224581.25</v>
       </c>
@@ -11234,7 +11241,7 @@
       <c r="A92" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B92" s="8">
+      <c r="B92" s="18">
         <f t="shared" si="1"/>
         <v>393300.5</v>
       </c>
@@ -11346,7 +11353,7 @@
       <c r="A93" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B93" s="8">
+      <c r="B93" s="18">
         <f t="shared" si="1"/>
         <v>279549.375</v>
       </c>
@@ -11458,7 +11465,7 @@
       <c r="A94" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B94" s="8">
+      <c r="B94" s="18">
         <f t="shared" si="1"/>
         <v>207150</v>
       </c>
@@ -11570,7 +11577,7 @@
       <c r="A95" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B95" s="8">
+      <c r="B95" s="18">
         <f t="shared" si="1"/>
         <v>212165.5</v>
       </c>
@@ -11682,7 +11689,7 @@
       <c r="A96" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B96" s="8">
+      <c r="B96" s="18">
         <f t="shared" si="1"/>
         <v>197406.25</v>
       </c>
@@ -11794,7 +11801,7 @@
       <c r="A97" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B97" s="8">
+      <c r="B97" s="18">
         <f t="shared" si="1"/>
         <v>415463.5</v>
       </c>
@@ -11906,7 +11913,7 @@
       <c r="A98" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B98" s="8">
+      <c r="B98" s="18">
         <f t="shared" si="1"/>
         <v>260000</v>
       </c>
@@ -12018,7 +12025,7 @@
       <c r="A99" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B99" s="8">
+      <c r="B99" s="18">
         <f t="shared" si="1"/>
         <v>475234.375</v>
       </c>
@@ -12130,7 +12137,7 @@
       <c r="A100" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B100" s="8">
+      <c r="B100" s="18">
         <f t="shared" si="1"/>
         <v>279700</v>
       </c>
@@ -12242,7 +12249,7 @@
       <c r="A101" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B101" s="8">
+      <c r="B101" s="18">
         <f t="shared" si="1"/>
         <v>344823.75</v>
       </c>
@@ -12354,7 +12361,7 @@
       <c r="A102" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B102" s="8">
+      <c r="B102" s="18">
         <f t="shared" si="1"/>
         <v>575835</v>
       </c>
@@ -12466,7 +12473,7 @@
       <c r="A103" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B103" s="8">
+      <c r="B103" s="18">
         <f t="shared" si="1"/>
         <v>218018.75</v>
       </c>
@@ -12578,7 +12585,7 @@
       <c r="A104" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B104" s="8">
+      <c r="B104" s="18">
         <f t="shared" si="1"/>
         <v>261175</v>
       </c>
@@ -12690,7 +12697,7 @@
       <c r="A105" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B105" s="8">
+      <c r="B105" s="18">
         <f t="shared" si="1"/>
         <v>808115.625</v>
       </c>
@@ -12802,7 +12809,7 @@
       <c r="A106" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B106" s="8">
+      <c r="B106" s="18">
         <f t="shared" si="1"/>
         <v>374675</v>
       </c>
@@ -12914,7 +12921,7 @@
       <c r="A107" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B107" s="8">
+      <c r="B107" s="18">
         <f t="shared" si="1"/>
         <v>309332.5</v>
       </c>
@@ -13026,7 +13033,7 @@
       <c r="A108" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B108" s="8">
+      <c r="B108" s="18">
         <f t="shared" si="1"/>
         <v>224214.5</v>
       </c>
@@ -13138,7 +13145,7 @@
       <c r="A109" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B109" s="8">
+      <c r="B109" s="18">
         <f t="shared" si="1"/>
         <v>326618.75</v>
       </c>
@@ -13250,7 +13257,7 @@
       <c r="A110" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B110" s="8">
+      <c r="B110" s="18">
         <f t="shared" si="1"/>
         <v>322120.625</v>
       </c>
@@ -13362,7 +13369,7 @@
       <c r="A111" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B111" s="8">
+      <c r="B111" s="18">
         <f t="shared" si="1"/>
         <v>348281.25</v>
       </c>
@@ -13474,7 +13481,7 @@
       <c r="A112" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B112" s="8">
+      <c r="B112" s="18">
         <f t="shared" si="1"/>
         <v>175175</v>
       </c>
@@ -13586,7 +13593,7 @@
       <c r="A113" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B113" s="8">
+      <c r="B113" s="18">
         <f t="shared" si="1"/>
         <v>264646.875</v>
       </c>
@@ -13698,7 +13705,7 @@
       <c r="A114" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B114" s="8">
+      <c r="B114" s="18">
         <f t="shared" si="1"/>
         <v>193468.33333333334</v>
       </c>
@@ -13810,7 +13817,7 @@
       <c r="A115" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B115" s="8">
+      <c r="B115" s="18">
         <f t="shared" si="1"/>
         <v>320671.875</v>
       </c>
@@ -13922,7 +13929,7 @@
       <c r="A116" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B116" s="8">
+      <c r="B116" s="18">
         <f t="shared" si="1"/>
         <v>171275</v>
       </c>
@@ -14034,7 +14041,7 @@
       <c r="A117" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B117" s="8">
+      <c r="B117" s="18">
         <f t="shared" si="1"/>
         <v>246175</v>
       </c>
@@ -14146,7 +14153,7 @@
       <c r="A118" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B118" s="8">
+      <c r="B118" s="18">
         <f t="shared" si="1"/>
         <v>447281.25</v>
       </c>
@@ -14258,7 +14265,7 @@
       <c r="A119" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B119" s="8">
+      <c r="B119" s="18">
         <f t="shared" si="1"/>
         <v>519681.25</v>
       </c>
@@ -14370,7 +14377,7 @@
       <c r="A120" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B120" s="8">
+      <c r="B120" s="18">
         <f t="shared" si="1"/>
         <v>289375</v>
       </c>
@@ -14482,7 +14489,7 @@
       <c r="A121" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B121" s="8">
+      <c r="B121" s="18">
         <f t="shared" si="1"/>
         <v>387466.625</v>
       </c>
@@ -14594,7 +14601,7 @@
       <c r="A122" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B122" s="8">
+      <c r="B122" s="18">
         <f t="shared" si="1"/>
         <v>296928.57142857142</v>
       </c>
@@ -14706,7 +14713,7 @@
       <c r="A123" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B123" s="8">
+      <c r="B123" s="18">
         <f t="shared" si="1"/>
         <v>221840.375</v>
       </c>
@@ -14818,7 +14825,7 @@
       <c r="A124" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B124" s="8">
+      <c r="B124" s="18">
         <f t="shared" si="1"/>
         <v>134331.25</v>
       </c>
@@ -14930,7 +14937,7 @@
       <c r="A125" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B125" s="8">
+      <c r="B125" s="18">
         <f t="shared" si="1"/>
         <v>382561.25</v>
       </c>
@@ -15042,7 +15049,7 @@
       <c r="A126" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="8">
+      <c r="B126" s="18">
         <f t="shared" si="1"/>
         <v>378375</v>
       </c>
@@ -15154,7 +15161,7 @@
       <c r="A127" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B127" s="8">
+      <c r="B127" s="18">
         <f t="shared" si="1"/>
         <v>279137.5</v>
       </c>
@@ -15266,7 +15273,7 @@
       <c r="A128" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B128" s="8">
+      <c r="B128" s="18">
         <f t="shared" si="1"/>
         <v>280456</v>
       </c>
@@ -15378,7 +15385,7 @@
       <c r="A129" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B129" s="8">
+      <c r="B129" s="18">
         <f t="shared" si="1"/>
         <v>322545.875</v>
       </c>
@@ -15490,7 +15497,7 @@
       <c r="A130" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B130" s="8">
+      <c r="B130" s="18">
         <f t="shared" si="1"/>
         <v>398124.375</v>
       </c>
@@ -15602,7 +15609,7 @@
       <c r="A131" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B131" s="8">
+      <c r="B131" s="18">
         <f t="shared" ref="B131:B134" si="2">AVERAGE(CT131:DA131)</f>
         <v>365437.5</v>
       </c>
@@ -15714,7 +15721,7 @@
       <c r="A132" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B132" s="8">
+      <c r="B132" s="18">
         <f t="shared" si="2"/>
         <v>148300</v>
       </c>
@@ -15826,7 +15833,7 @@
       <c r="A133" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B133" s="8">
+      <c r="B133" s="18">
         <f t="shared" si="2"/>
         <v>209118.75</v>
       </c>
@@ -15938,7 +15945,7 @@
       <c r="A134" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B134" s="8">
+      <c r="B134" s="18">
         <f t="shared" si="2"/>
         <v>415045.375</v>
       </c>
@@ -16063,6 +16070,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18171fec-acf4-43d2-b526-0e7db5044e74">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fcf87922-c7f3-44a4-9aa8-f585f70d1698" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3EBF122F3DB854AB6515567219CA9AB" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95866c8e7206fe2ad6c1db40d1ce538a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18171fec-acf4-43d2-b526-0e7db5044e74" xmlns:ns3="fcf87922-c7f3-44a4-9aa8-f585f70d1698" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b9244ac4e6d70d4305f413f251a8df0d" ns2:_="" ns3:_="">
     <xsd:import namespace="18171fec-acf4-43d2-b526-0e7db5044e74"/>
@@ -16311,17 +16329,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18171fec-acf4-43d2-b526-0e7db5044e74">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fcf87922-c7f3-44a4-9aa8-f585f70d1698" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -16332,6 +16339,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDE6DCB8-39B5-4069-9C8C-C617590561FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18171fec-acf4-43d2-b526-0e7db5044e74"/>
+    <ds:schemaRef ds:uri="fcf87922-c7f3-44a4-9aa8-f585f70d1698"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2446006E-85E9-4E5E-98D3-13C3CF1C4B87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16350,17 +16368,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDE6DCB8-39B5-4069-9C8C-C617590561FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18171fec-acf4-43d2-b526-0e7db5044e74"/>
-    <ds:schemaRef ds:uri="fcf87922-c7f3-44a4-9aa8-f585f70d1698"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C0B4F78-785D-4059-A899-453621A39DE3}">
   <ds:schemaRefs>

</xml_diff>